<commit_message>
- Schéma du système de santé complété.
- maquette du 008
</commit_message>
<xml_diff>
--- a/thématique SI/007 SI et stratégie/storyboard 007.xlsx
+++ b/thématique SI/007 SI et stratégie/storyboard 007.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincent/Library/Mobile Documents/com~apple~CloudDocs/Documents/pro/ISIS/2023-2024/dev/projet-FENS/thématique SI/007 SI et stratégie/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71DE35F3-1AEB-1043-908A-6C4EA2F01553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E236A78E-9EF8-944A-949F-5C118DEBB599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1000" windowWidth="35680" windowHeight="21000" xr2:uid="{A4F29CA4-E8D0-5846-A34B-CC524442BAF9}"/>
+    <workbookView xWindow="15520" yWindow="440" windowWidth="38980" windowHeight="26060" xr2:uid="{A4F29CA4-E8D0-5846-A34B-CC524442BAF9}"/>
   </bookViews>
   <sheets>
     <sheet name="007" sheetId="9" r:id="rId1"/>
@@ -576,7 +576,7 @@
   <dimension ref="A2:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
{ADD} rsrc capsule 007
</commit_message>
<xml_diff>
--- a/thématique SI/007 SI et stratégie/storyboard 007.xlsx
+++ b/thématique SI/007 SI et stratégie/storyboard 007.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26505"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincent/Library/Mobile Documents/com~apple~CloudDocs/Documents/pro/ISIS/2023-2024/dev/projet-FENS/thématique SI/007 SI et stratégie/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stage\projet-FENS\thématique SI\007 SI et stratégie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E236A78E-9EF8-944A-949F-5C118DEBB599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48A778E-B3E0-4C98-85C0-416C3E9652F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15520" yWindow="440" windowWidth="38980" windowHeight="26060" xr2:uid="{A4F29CA4-E8D0-5846-A34B-CC524442BAF9}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{A4F29CA4-E8D0-5846-A34B-CC524442BAF9}"/>
   </bookViews>
   <sheets>
     <sheet name="007" sheetId="9" r:id="rId1"/>
@@ -20,14 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -83,9 +75,6 @@
     <t>Savoir ce qu'est un schéma directeur</t>
   </si>
   <si>
-    <t>Terme issu du domaine militaire, la stratégie revient à choisir contre qui on se bat et pour quelle cause.</t>
-  </si>
-  <si>
     <t>Les investissement lourds, les coûts de fonctionnement élevés, les durées importantes des tâches, nécessitent d'anticiper sur du long terme.
 Définir une stratégie est alors nécessaire.</t>
   </si>
@@ -107,9 +96,6 @@
   <si>
     <t>La stratégie est un plan global qui fixe des axes directeurs.
 Ce sont des lignes directrices qui vont guider les décisions et les actions.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Formation, analyse d'affaire, achat de logiciel, matériel, dématérialisation, évolution des métiers; toutes les couches du S.I. sont concernées. </t>
   </si>
   <si>
     <t>Ce document de référence permet d'évaluer et de retenir, ou non, les futures opportunités d'évolution du portefeuille des projets S.I.. Comme toutes les couches sont concernées, ceci inclut les évolutions matérielles, logicielles, fonctionnelles et métier.</t>
@@ -131,6 +117,12 @@
 - Gestion des risques d’un projet SI :
 organigramme des risques et analyse
 Pilotage opérationnel :</t>
+  </si>
+  <si>
+    <t>La stratégie est un terme issu du domaine militaire, elle revient à choisir contre qui on se bat et pour quelle cause.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On peut citer comme exemple d’axes directeurs : une formation, une analyse d'affaire, un achat de logiciel, un matériel, une dématérialisation, une évolution des métiers; ainsi toutes les couches du S.I. sont concernées. </t>
   </si>
 </sst>
 </file>
@@ -223,7 +215,7 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>3654135</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>289790</xdr:rowOff>
+      <xdr:rowOff>282170</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -575,20 +567,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D12403-33F0-BA47-A116-4D02C2D6DFDE}">
   <dimension ref="A2:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="2" max="2" width="52.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="49.83203125" customWidth="1"/>
-    <col min="4" max="4" width="40.83203125" customWidth="1"/>
+    <col min="1" max="1" width="25.296875" customWidth="1"/>
+    <col min="2" max="2" width="52.19921875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="49.796875" customWidth="1"/>
+    <col min="4" max="4" width="40.796875" customWidth="1"/>
     <col min="6" max="6" width="36.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -596,17 +588,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>3</v>
       </c>
@@ -620,44 +612,44 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="B12" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="B13" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="B14" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" t="s">
         <v>4</v>
@@ -666,34 +658,34 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="204" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D18" s="1"/>
       <c r="F18" s="1" t="s">

</xml_diff>

<commit_message>
meilleur suivi de la nomenclature
</commit_message>
<xml_diff>
--- a/thématique SI/007 SI et stratégie/storyboard 007.xlsx
+++ b/thématique SI/007 SI et stratégie/storyboard 007.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26505"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stage\projet-FENS\thématique SI\007 SI et stratégie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincent/Documents/dev/projet-FENS/thématique SI/007 SI et stratégie/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48A778E-B3E0-4C98-85C0-416C3E9652F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F196277-8E67-9A4F-9805-2785D01B01F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{A4F29CA4-E8D0-5846-A34B-CC524442BAF9}"/>
+    <workbookView xWindow="4640" yWindow="980" windowWidth="26080" windowHeight="15020" xr2:uid="{A4F29CA4-E8D0-5846-A34B-CC524442BAF9}"/>
   </bookViews>
   <sheets>
     <sheet name="007" sheetId="9" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Objectif</t>
   </si>
@@ -75,10 +75,6 @@
     <t>Savoir ce qu'est un schéma directeur</t>
   </si>
   <si>
-    <t>Les investissement lourds, les coûts de fonctionnement élevés, les durées importantes des tâches, nécessitent d'anticiper sur du long terme.
-Définir une stratégie est alors nécessaire.</t>
-  </si>
-  <si>
     <t>Besoin d'un stratégie</t>
   </si>
   <si>
@@ -92,10 +88,6 @@
   </si>
   <si>
     <t>Chaque axe directeur va donner naissance à des idées de projet,  qui selon leur balance bénéfice-risque, seront inclus dans le "schéma directeur du Système d'information".</t>
-  </si>
-  <si>
-    <t>La stratégie est un plan global qui fixe des axes directeurs.
-Ce sont des lignes directrices qui vont guider les décisions et les actions.</t>
   </si>
   <si>
     <t>Ce document de référence permet d'évaluer et de retenir, ou non, les futures opportunités d'évolution du portefeuille des projets S.I.. Comme toutes les couches sont concernées, ceci inclut les évolutions matérielles, logicielles, fonctionnelles et métier.</t>
@@ -124,12 +116,44 @@
   <si>
     <t xml:space="preserve">On peut citer comme exemple d’axes directeurs : une formation, une analyse d'affaire, un achat de logiciel, un matériel, une dématérialisation, une évolution des métiers; ainsi toutes les couches du S.I. sont concernées. </t>
   </si>
+  <si>
+    <t>c010</t>
+  </si>
+  <si>
+    <t>c020</t>
+  </si>
+  <si>
+    <t>c030</t>
+  </si>
+  <si>
+    <t>c040</t>
+  </si>
+  <si>
+    <t>c050</t>
+  </si>
+  <si>
+    <t>c060</t>
+  </si>
+  <si>
+    <t>c070</t>
+  </si>
+  <si>
+    <t>c080</t>
+  </si>
+  <si>
+    <t>Les investissement lourds, les coûts de fonctionnement élevés, les durées importantes des tâches, nécessitent d'anticiper sur le pilotage au long terme.
+Définir une stratégie est alors nécessaire.</t>
+  </si>
+  <si>
+    <t>C'est un plan global qui fixe des axes directeurs.
+Ce sont des lignes directrices qui vont guider les décisions et les actions.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -148,6 +172,12 @@
     <font>
       <sz val="12"/>
       <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -206,13 +236,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>889000</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>22048</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>3654135</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>282170</xdr:rowOff>
@@ -565,134 +595,159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D12403-33F0-BA47-A116-4D02C2D6DFDE}">
-  <dimension ref="A2:F18"/>
+  <dimension ref="A2:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="186" zoomScaleNormal="186" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.296875" customWidth="1"/>
-    <col min="2" max="2" width="52.19921875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="49.796875" customWidth="1"/>
-    <col min="4" max="4" width="40.796875" customWidth="1"/>
-    <col min="6" max="6" width="36.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="53" style="1" customWidth="1"/>
+    <col min="4" max="4" width="49.83203125" customWidth="1"/>
+    <col min="5" max="5" width="40.83203125" customWidth="1"/>
+    <col min="7" max="7" width="36.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
+    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
         <v>3</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>10</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="C12" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+      <c r="C13" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="C14" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" t="s">
-        <v>4</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="109.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="4" t="s">
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="204" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="F18" s="1" t="s">
+      <c r="E18" s="1"/>
+      <c r="G18" s="1" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>